<commit_message>
#8466 - remove some ITU indicators
</commit_message>
<xml_diff>
--- a/db/sources.xlsx
+++ b/db/sources.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="484">
   <si>
     <t>Include in Internet Monitor?</t>
   </si>
@@ -2327,8 +2327,8 @@
   <dimension ref="A1:AF145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K16" sqref="K16"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3434,9 +3434,6 @@
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
       <c r="B26" t="s">
         <v>31</v>
       </c>
@@ -3487,9 +3484,6 @@
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
       <c r="B27" t="s">
         <v>31</v>
       </c>
@@ -3546,9 +3540,6 @@
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
       <c r="K28" t="s">
         <v>128</v>
       </c>
@@ -3596,9 +3587,6 @@
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
       <c r="J29" t="s">
         <v>31</v>
       </c>
@@ -4292,189 +4280,366 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" t="s">
+        <v>31</v>
+      </c>
+      <c r="I49">
+        <v>100</v>
+      </c>
       <c r="K49" t="s">
+        <v>454</v>
+      </c>
+      <c r="L49" t="s">
+        <v>455</v>
+      </c>
+      <c r="M49" t="s">
+        <v>456</v>
+      </c>
+      <c r="P49">
+        <v>2013</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>457</v>
+      </c>
+      <c r="R49" t="s">
+        <v>424</v>
+      </c>
+      <c r="S49" t="s">
+        <v>39</v>
+      </c>
+      <c r="U49">
+        <v>1</v>
+      </c>
+      <c r="V49" t="s">
+        <v>40</v>
+      </c>
+      <c r="W49" t="s">
+        <v>125</v>
+      </c>
+      <c r="X49" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>459</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>460</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>461</v>
+      </c>
+      <c r="AD49" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>31</v>
+      </c>
+      <c r="H50" t="s">
+        <v>31</v>
+      </c>
+      <c r="I50">
+        <v>100</v>
+      </c>
+      <c r="K50" t="s">
+        <v>463</v>
+      </c>
+      <c r="L50" t="s">
+        <v>464</v>
+      </c>
+      <c r="M50" t="s">
+        <v>456</v>
+      </c>
+      <c r="P50">
+        <v>2013</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>457</v>
+      </c>
+      <c r="R50" t="s">
+        <v>424</v>
+      </c>
+      <c r="S50" t="s">
+        <v>39</v>
+      </c>
+      <c r="U50">
+        <v>1</v>
+      </c>
+      <c r="V50" t="s">
+        <v>40</v>
+      </c>
+      <c r="W50" t="s">
+        <v>125</v>
+      </c>
+      <c r="X50" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>465</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>466</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>461</v>
+      </c>
+      <c r="AD50" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" t="s">
+        <v>31</v>
+      </c>
+      <c r="I51">
+        <v>100</v>
+      </c>
+      <c r="K51" t="s">
+        <v>467</v>
+      </c>
+      <c r="L51" t="s">
+        <v>468</v>
+      </c>
+      <c r="M51" t="s">
+        <v>456</v>
+      </c>
+      <c r="P51">
+        <v>2013</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>457</v>
+      </c>
+      <c r="R51" t="s">
+        <v>424</v>
+      </c>
+      <c r="S51" t="s">
+        <v>39</v>
+      </c>
+      <c r="U51">
+        <v>1</v>
+      </c>
+      <c r="V51" t="s">
+        <v>40</v>
+      </c>
+      <c r="W51" t="s">
+        <v>125</v>
+      </c>
+      <c r="X51" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>469</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>470</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>461</v>
+      </c>
+      <c r="AD51" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>31</v>
+      </c>
+      <c r="H52" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52">
+        <v>100</v>
+      </c>
+      <c r="K52" t="s">
+        <v>471</v>
+      </c>
+      <c r="L52" t="s">
+        <v>472</v>
+      </c>
+      <c r="M52" t="s">
+        <v>456</v>
+      </c>
+      <c r="P52">
+        <v>2013</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>457</v>
+      </c>
+      <c r="R52" t="s">
+        <v>424</v>
+      </c>
+      <c r="S52" t="s">
+        <v>39</v>
+      </c>
+      <c r="U52">
+        <v>1</v>
+      </c>
+      <c r="V52" t="s">
+        <v>40</v>
+      </c>
+      <c r="W52" t="s">
+        <v>125</v>
+      </c>
+      <c r="X52" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>473</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>461</v>
+      </c>
+      <c r="AD52" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>31</v>
+      </c>
+      <c r="H53" t="s">
+        <v>31</v>
+      </c>
+      <c r="I53">
+        <v>100</v>
+      </c>
+      <c r="K53" t="s">
+        <v>475</v>
+      </c>
+      <c r="L53" t="s">
+        <v>476</v>
+      </c>
+      <c r="M53" t="s">
+        <v>456</v>
+      </c>
+      <c r="P53">
+        <v>2013</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>457</v>
+      </c>
+      <c r="R53" t="s">
+        <v>424</v>
+      </c>
+      <c r="S53" t="s">
+        <v>39</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+      <c r="V53" t="s">
+        <v>40</v>
+      </c>
+      <c r="W53" t="s">
+        <v>125</v>
+      </c>
+      <c r="X53" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>477</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>478</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>461</v>
+      </c>
+      <c r="AD53" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="D54" t="s">
+        <v>121</v>
+      </c>
+      <c r="H54" t="s">
+        <v>31</v>
+      </c>
+      <c r="K54" t="s">
+        <v>479</v>
+      </c>
+      <c r="L54" t="s">
+        <v>480</v>
+      </c>
+      <c r="M54" t="s">
+        <v>456</v>
+      </c>
+      <c r="P54">
+        <v>2013</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>457</v>
+      </c>
+      <c r="R54" t="s">
+        <v>424</v>
+      </c>
+      <c r="S54" t="s">
+        <v>39</v>
+      </c>
+      <c r="U54">
+        <v>1</v>
+      </c>
+      <c r="V54" t="s">
+        <v>40</v>
+      </c>
+      <c r="W54" t="s">
+        <v>125</v>
+      </c>
+      <c r="X54" t="s">
+        <v>458</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>481</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>481</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>461</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
         <v>182</v>
       </c>
-      <c r="L49" t="s">
+      <c r="L55" t="s">
         <v>183</v>
-      </c>
-      <c r="M49" t="s">
-        <v>184</v>
-      </c>
-      <c r="N49" t="s">
-        <v>185</v>
-      </c>
-      <c r="O49" t="s">
-        <v>36</v>
-      </c>
-      <c r="P49">
-        <v>2011</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>186</v>
-      </c>
-      <c r="S49" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K50" t="s">
-        <v>187</v>
-      </c>
-      <c r="L50" t="s">
-        <v>188</v>
-      </c>
-      <c r="M50" t="s">
-        <v>184</v>
-      </c>
-      <c r="N50" t="s">
-        <v>185</v>
-      </c>
-      <c r="O50" t="s">
-        <v>36</v>
-      </c>
-      <c r="P50">
-        <v>2011</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>186</v>
-      </c>
-      <c r="S50" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K51" t="s">
-        <v>189</v>
-      </c>
-      <c r="L51" t="s">
-        <v>190</v>
-      </c>
-      <c r="M51" t="s">
-        <v>184</v>
-      </c>
-      <c r="N51" t="s">
-        <v>185</v>
-      </c>
-      <c r="O51" t="s">
-        <v>36</v>
-      </c>
-      <c r="P51">
-        <v>2011</v>
-      </c>
-      <c r="Q51" t="s">
-        <v>186</v>
-      </c>
-      <c r="S51" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>31</v>
-      </c>
-      <c r="K52" t="s">
-        <v>191</v>
-      </c>
-      <c r="L52" t="s">
-        <v>192</v>
-      </c>
-      <c r="M52" t="s">
-        <v>184</v>
-      </c>
-      <c r="N52" t="s">
-        <v>185</v>
-      </c>
-      <c r="O52" t="s">
-        <v>36</v>
-      </c>
-      <c r="P52">
-        <v>2011</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>186</v>
-      </c>
-      <c r="S52" t="s">
-        <v>39</v>
-      </c>
-      <c r="U52">
-        <v>-1</v>
-      </c>
-      <c r="V52" t="s">
-        <v>193</v>
-      </c>
-      <c r="W52" t="s">
-        <v>194</v>
-      </c>
-      <c r="X52" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z52" t="s">
-        <v>196</v>
-      </c>
-      <c r="AB52" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K53" t="s">
-        <v>198</v>
-      </c>
-      <c r="L53" t="s">
-        <v>199</v>
-      </c>
-      <c r="M53" t="s">
-        <v>184</v>
-      </c>
-      <c r="N53" t="s">
-        <v>185</v>
-      </c>
-      <c r="O53" t="s">
-        <v>36</v>
-      </c>
-      <c r="P53">
-        <v>2011</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>186</v>
-      </c>
-      <c r="S53" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K54" t="s">
-        <v>200</v>
-      </c>
-      <c r="L54" t="s">
-        <v>201</v>
-      </c>
-      <c r="M54" t="s">
-        <v>184</v>
-      </c>
-      <c r="N54" t="s">
-        <v>185</v>
-      </c>
-      <c r="O54" t="s">
-        <v>36</v>
-      </c>
-      <c r="P54">
-        <v>2011</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>186</v>
-      </c>
-      <c r="S54" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K55" t="s">
-        <v>202</v>
-      </c>
-      <c r="L55" t="s">
-        <v>203</v>
       </c>
       <c r="M55" t="s">
         <v>184</v>
@@ -4495,7 +4660,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>187</v>
+      </c>
+      <c r="L56" t="s">
+        <v>188</v>
+      </c>
       <c r="M56" t="s">
         <v>184</v>
       </c>
@@ -4508,209 +4679,182 @@
       <c r="P56">
         <v>2011</v>
       </c>
+      <c r="Q56" t="s">
+        <v>186</v>
+      </c>
       <c r="S56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
+        <v>189</v>
+      </c>
+      <c r="L57" t="s">
+        <v>190</v>
+      </c>
+      <c r="M57" t="s">
+        <v>184</v>
+      </c>
+      <c r="N57" t="s">
+        <v>185</v>
+      </c>
+      <c r="O57" t="s">
+        <v>36</v>
+      </c>
+      <c r="P57">
+        <v>2011</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>186</v>
+      </c>
+      <c r="S57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>31</v>
+      </c>
+      <c r="K58" t="s">
+        <v>191</v>
+      </c>
+      <c r="L58" t="s">
+        <v>192</v>
+      </c>
+      <c r="M58" t="s">
+        <v>184</v>
+      </c>
+      <c r="N58" t="s">
+        <v>185</v>
+      </c>
+      <c r="O58" t="s">
+        <v>36</v>
+      </c>
+      <c r="P58">
+        <v>2011</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>186</v>
+      </c>
+      <c r="S58" t="s">
+        <v>39</v>
+      </c>
+      <c r="U58">
+        <v>-1</v>
+      </c>
+      <c r="V58" t="s">
+        <v>193</v>
+      </c>
+      <c r="W58" t="s">
+        <v>194</v>
+      </c>
+      <c r="X58" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>196</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>198</v>
+      </c>
+      <c r="L59" t="s">
+        <v>199</v>
+      </c>
+      <c r="M59" t="s">
+        <v>184</v>
+      </c>
+      <c r="N59" t="s">
+        <v>185</v>
+      </c>
+      <c r="O59" t="s">
+        <v>36</v>
+      </c>
+      <c r="P59">
+        <v>2011</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>186</v>
+      </c>
+      <c r="S59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K60" t="s">
+        <v>200</v>
+      </c>
+      <c r="L60" t="s">
+        <v>201</v>
+      </c>
+      <c r="M60" t="s">
+        <v>184</v>
+      </c>
+      <c r="N60" t="s">
+        <v>185</v>
+      </c>
+      <c r="O60" t="s">
+        <v>36</v>
+      </c>
+      <c r="P60">
+        <v>2011</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>186</v>
+      </c>
+      <c r="S60" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K61" t="s">
+        <v>202</v>
+      </c>
+      <c r="L61" t="s">
+        <v>203</v>
+      </c>
+      <c r="M61" t="s">
+        <v>184</v>
+      </c>
+      <c r="N61" t="s">
+        <v>185</v>
+      </c>
+      <c r="O61" t="s">
+        <v>36</v>
+      </c>
+      <c r="P61">
+        <v>2011</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>186</v>
+      </c>
+      <c r="S61" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="M62" t="s">
+        <v>184</v>
+      </c>
+      <c r="N62" t="s">
+        <v>185</v>
+      </c>
+      <c r="O62" t="s">
+        <v>36</v>
+      </c>
+      <c r="P62">
+        <v>2011</v>
+      </c>
+      <c r="S62" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="M57" t="s">
-        <v>205</v>
-      </c>
-      <c r="N57" t="s">
-        <v>206</v>
-      </c>
-      <c r="O57" t="s">
-        <v>36</v>
-      </c>
-      <c r="P57" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q57" t="s">
-        <v>208</v>
-      </c>
-      <c r="S57" t="s">
-        <v>39</v>
-      </c>
-      <c r="T57" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="M58" t="s">
-        <v>205</v>
-      </c>
-      <c r="N58" t="s">
-        <v>206</v>
-      </c>
-      <c r="O58" t="s">
-        <v>36</v>
-      </c>
-      <c r="P58" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q58" t="s">
-        <v>208</v>
-      </c>
-      <c r="S58" t="s">
-        <v>39</v>
-      </c>
-      <c r="T58" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>31</v>
-      </c>
-      <c r="B59" t="s">
-        <v>31</v>
-      </c>
-      <c r="K59" t="s">
-        <v>210</v>
-      </c>
-      <c r="L59" t="s">
-        <v>211</v>
-      </c>
-      <c r="M59" t="s">
-        <v>205</v>
-      </c>
-      <c r="N59" t="s">
-        <v>206</v>
-      </c>
-      <c r="O59" t="s">
-        <v>36</v>
-      </c>
-      <c r="P59" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>212</v>
-      </c>
-      <c r="S59" t="s">
-        <v>39</v>
-      </c>
-      <c r="T59" t="s">
-        <v>209</v>
-      </c>
-      <c r="U59">
-        <v>1</v>
-      </c>
-      <c r="V59" t="s">
-        <v>40</v>
-      </c>
-      <c r="W59" t="s">
-        <v>41</v>
-      </c>
-      <c r="X59" t="s">
-        <v>213</v>
-      </c>
-      <c r="Z59" t="s">
-        <v>214</v>
-      </c>
-      <c r="AB59" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K60" t="s">
-        <v>216</v>
-      </c>
-      <c r="L60" t="s">
-        <v>217</v>
-      </c>
-      <c r="M60" t="s">
-        <v>205</v>
-      </c>
-      <c r="N60" t="s">
-        <v>206</v>
-      </c>
-      <c r="O60" t="s">
-        <v>36</v>
-      </c>
-      <c r="P60" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>212</v>
-      </c>
-      <c r="S60" t="s">
-        <v>39</v>
-      </c>
-      <c r="T60" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K61" t="s">
-        <v>218</v>
-      </c>
-      <c r="L61" t="s">
-        <v>219</v>
-      </c>
-      <c r="M61" t="s">
-        <v>205</v>
-      </c>
-      <c r="N61" t="s">
-        <v>206</v>
-      </c>
-      <c r="O61" t="s">
-        <v>36</v>
-      </c>
-      <c r="P61" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>212</v>
-      </c>
-      <c r="S61" t="s">
-        <v>39</v>
-      </c>
-      <c r="T61" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="K62" t="s">
-        <v>220</v>
-      </c>
-      <c r="L62" t="s">
-        <v>221</v>
-      </c>
-      <c r="M62" t="s">
-        <v>205</v>
-      </c>
-      <c r="N62" t="s">
-        <v>206</v>
-      </c>
-      <c r="O62" t="s">
-        <v>36</v>
-      </c>
-      <c r="P62" t="s">
-        <v>207</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>212</v>
-      </c>
-      <c r="S62" t="s">
-        <v>39</v>
-      </c>
-      <c r="T62" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>31</v>
-      </c>
-      <c r="B63" t="s">
-        <v>31</v>
-      </c>
-      <c r="K63" t="s">
-        <v>222</v>
-      </c>
-      <c r="L63" t="s">
-        <v>223</v>
-      </c>
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="M63" t="s">
         <v>205</v>
       </c>
@@ -4724,7 +4868,7 @@
         <v>207</v>
       </c>
       <c r="Q63" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="S63" t="s">
         <v>39</v>
@@ -4732,41 +4876,8 @@
       <c r="T63" t="s">
         <v>209</v>
       </c>
-      <c r="U63">
-        <v>1</v>
-      </c>
-      <c r="V63" t="s">
-        <v>40</v>
-      </c>
-      <c r="W63" t="s">
-        <v>41</v>
-      </c>
-      <c r="X63" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z63" t="s">
-        <v>226</v>
-      </c>
-      <c r="AB63" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD63" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" t="s">
-        <v>31</v>
-      </c>
-      <c r="K64" t="s">
-        <v>227</v>
-      </c>
-      <c r="L64" t="s">
-        <v>228</v>
-      </c>
+    </row>
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="M64" t="s">
         <v>205</v>
       </c>
@@ -4780,7 +4891,7 @@
         <v>207</v>
       </c>
       <c r="Q64" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="S64" t="s">
         <v>39</v>
@@ -4788,29 +4899,20 @@
       <c r="T64" t="s">
         <v>209</v>
       </c>
-      <c r="U64">
-        <v>1</v>
-      </c>
-      <c r="V64" t="s">
-        <v>40</v>
-      </c>
-      <c r="W64" t="s">
-        <v>41</v>
-      </c>
-      <c r="X64" t="s">
-        <v>225</v>
-      </c>
-      <c r="Z64" t="s">
-        <v>229</v>
-      </c>
-      <c r="AB64" t="s">
-        <v>215</v>
-      </c>
-      <c r="AD64" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="65" spans="11:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" t="s">
+        <v>31</v>
+      </c>
+      <c r="K65" t="s">
+        <v>210</v>
+      </c>
+      <c r="L65" t="s">
+        <v>211</v>
+      </c>
       <c r="M65" t="s">
         <v>205</v>
       </c>
@@ -4824,7 +4926,7 @@
         <v>207</v>
       </c>
       <c r="Q65" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="S65" t="s">
         <v>39</v>
@@ -4832,8 +4934,32 @@
       <c r="T65" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="66" spans="11:20" x14ac:dyDescent="0.25">
+      <c r="U65">
+        <v>1</v>
+      </c>
+      <c r="V65" t="s">
+        <v>40</v>
+      </c>
+      <c r="W65" t="s">
+        <v>41</v>
+      </c>
+      <c r="X65" t="s">
+        <v>213</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="K66" t="s">
+        <v>216</v>
+      </c>
+      <c r="L66" t="s">
+        <v>217</v>
+      </c>
       <c r="M66" t="s">
         <v>205</v>
       </c>
@@ -4847,7 +4973,7 @@
         <v>207</v>
       </c>
       <c r="Q66" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="S66" t="s">
         <v>39</v>
@@ -4856,168 +4982,228 @@
         <v>209</v>
       </c>
     </row>
-    <row r="67" spans="11:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K67" t="s">
+        <v>218</v>
+      </c>
+      <c r="L67" t="s">
+        <v>219</v>
+      </c>
+      <c r="M67" t="s">
+        <v>205</v>
+      </c>
+      <c r="N67" t="s">
+        <v>206</v>
+      </c>
+      <c r="O67" t="s">
+        <v>36</v>
+      </c>
+      <c r="P67" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>212</v>
+      </c>
+      <c r="S67" t="s">
+        <v>39</v>
+      </c>
+      <c r="T67" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
+        <v>220</v>
+      </c>
+      <c r="L68" t="s">
+        <v>221</v>
+      </c>
+      <c r="M68" t="s">
+        <v>205</v>
+      </c>
+      <c r="N68" t="s">
+        <v>206</v>
+      </c>
+      <c r="O68" t="s">
+        <v>36</v>
+      </c>
+      <c r="P68" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>212</v>
+      </c>
+      <c r="S68" t="s">
+        <v>39</v>
+      </c>
+      <c r="T68" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" t="s">
+        <v>31</v>
+      </c>
+      <c r="K69" t="s">
+        <v>222</v>
+      </c>
+      <c r="L69" t="s">
+        <v>223</v>
+      </c>
+      <c r="M69" t="s">
+        <v>205</v>
+      </c>
+      <c r="N69" t="s">
+        <v>206</v>
+      </c>
+      <c r="O69" t="s">
+        <v>36</v>
+      </c>
+      <c r="P69" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>224</v>
+      </c>
+      <c r="S69" t="s">
+        <v>39</v>
+      </c>
+      <c r="T69" t="s">
+        <v>209</v>
+      </c>
+      <c r="U69">
+        <v>1</v>
+      </c>
+      <c r="V69" t="s">
+        <v>40</v>
+      </c>
+      <c r="W69" t="s">
+        <v>41</v>
+      </c>
+      <c r="X69" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" t="s">
+        <v>31</v>
+      </c>
+      <c r="K70" t="s">
+        <v>227</v>
+      </c>
+      <c r="L70" t="s">
+        <v>228</v>
+      </c>
+      <c r="M70" t="s">
+        <v>205</v>
+      </c>
+      <c r="N70" t="s">
+        <v>206</v>
+      </c>
+      <c r="O70" t="s">
+        <v>36</v>
+      </c>
+      <c r="P70" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>224</v>
+      </c>
+      <c r="S70" t="s">
+        <v>39</v>
+      </c>
+      <c r="T70" t="s">
+        <v>209</v>
+      </c>
+      <c r="U70">
+        <v>1</v>
+      </c>
+      <c r="V70" t="s">
+        <v>40</v>
+      </c>
+      <c r="W70" t="s">
+        <v>41</v>
+      </c>
+      <c r="X70" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB70" t="s">
+        <v>215</v>
+      </c>
+      <c r="AD70" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M71" t="s">
+        <v>205</v>
+      </c>
+      <c r="N71" t="s">
+        <v>206</v>
+      </c>
+      <c r="O71" t="s">
+        <v>36</v>
+      </c>
+      <c r="P71" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>230</v>
+      </c>
+      <c r="S71" t="s">
+        <v>39</v>
+      </c>
+      <c r="T71" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M72" t="s">
+        <v>205</v>
+      </c>
+      <c r="N72" t="s">
+        <v>206</v>
+      </c>
+      <c r="O72" t="s">
+        <v>36</v>
+      </c>
+      <c r="P72" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>230</v>
+      </c>
+      <c r="S72" t="s">
+        <v>39</v>
+      </c>
+      <c r="T72" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="K73" t="s">
         <v>231</v>
       </c>
-      <c r="L67" t="s">
+      <c r="L73" t="s">
         <v>232</v>
-      </c>
-      <c r="M67" t="s">
-        <v>233</v>
-      </c>
-      <c r="N67" t="s">
-        <v>234</v>
-      </c>
-      <c r="O67" t="s">
-        <v>36</v>
-      </c>
-      <c r="P67" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>236</v>
-      </c>
-      <c r="S67" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="68" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K68" t="s">
-        <v>237</v>
-      </c>
-      <c r="L68" t="s">
-        <v>238</v>
-      </c>
-      <c r="M68" t="s">
-        <v>233</v>
-      </c>
-      <c r="N68" t="s">
-        <v>234</v>
-      </c>
-      <c r="O68" t="s">
-        <v>36</v>
-      </c>
-      <c r="P68" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>236</v>
-      </c>
-      <c r="S68" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="69" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K69" t="s">
-        <v>239</v>
-      </c>
-      <c r="L69" t="s">
-        <v>240</v>
-      </c>
-      <c r="M69" t="s">
-        <v>233</v>
-      </c>
-      <c r="N69" t="s">
-        <v>234</v>
-      </c>
-      <c r="O69" t="s">
-        <v>36</v>
-      </c>
-      <c r="P69" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>236</v>
-      </c>
-      <c r="S69" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="70" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K70" t="s">
-        <v>241</v>
-      </c>
-      <c r="L70" t="s">
-        <v>242</v>
-      </c>
-      <c r="M70" t="s">
-        <v>233</v>
-      </c>
-      <c r="N70" t="s">
-        <v>234</v>
-      </c>
-      <c r="O70" t="s">
-        <v>36</v>
-      </c>
-      <c r="P70" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>236</v>
-      </c>
-      <c r="S70" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K71" t="s">
-        <v>243</v>
-      </c>
-      <c r="L71" t="s">
-        <v>244</v>
-      </c>
-      <c r="M71" t="s">
-        <v>233</v>
-      </c>
-      <c r="N71" t="s">
-        <v>234</v>
-      </c>
-      <c r="O71" t="s">
-        <v>36</v>
-      </c>
-      <c r="P71" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>236</v>
-      </c>
-      <c r="S71" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="72" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K72" t="s">
-        <v>245</v>
-      </c>
-      <c r="L72" t="s">
-        <v>246</v>
-      </c>
-      <c r="M72" t="s">
-        <v>233</v>
-      </c>
-      <c r="N72" t="s">
-        <v>234</v>
-      </c>
-      <c r="O72" t="s">
-        <v>36</v>
-      </c>
-      <c r="P72" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>236</v>
-      </c>
-      <c r="S72" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="73" spans="11:20" x14ac:dyDescent="0.25">
-      <c r="K73" t="s">
-        <v>247</v>
-      </c>
-      <c r="L73" t="s">
-        <v>248</v>
       </c>
       <c r="M73" t="s">
         <v>233</v>
@@ -5038,12 +5224,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="11:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K74" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="L74" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="M74" t="s">
         <v>233</v>
@@ -5064,12 +5250,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="11:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K75" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="L75" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="M75" t="s">
         <v>233</v>
@@ -5090,12 +5276,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="76" spans="11:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K76" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="L76" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="M76" t="s">
         <v>233</v>
@@ -5116,12 +5302,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="77" spans="11:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K77" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="L77" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="M77" t="s">
         <v>233</v>
@@ -5142,12 +5328,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="78" spans="11:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K78" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="L78" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="M78" t="s">
         <v>233</v>
@@ -5168,12 +5354,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="11:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K79" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="L79" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="M79" t="s">
         <v>233</v>
@@ -5194,12 +5380,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="80" spans="11:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.25">
       <c r="K80" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="L80" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="M80" t="s">
         <v>233</v>
@@ -5220,12 +5406,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="81" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K81" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="L81" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="M81" t="s">
         <v>233</v>
@@ -5246,12 +5432,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="82" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K82" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="L82" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="M82" t="s">
         <v>233</v>
@@ -5272,12 +5458,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="83" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K83" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="L83" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="M83" t="s">
         <v>233</v>
@@ -5298,12 +5484,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="84" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K84" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="L84" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="M84" t="s">
         <v>233</v>
@@ -5324,12 +5510,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="85" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K85" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="L85" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="M85" t="s">
         <v>233</v>
@@ -5350,12 +5536,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="86" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K86" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="L86" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="M86" t="s">
         <v>233</v>
@@ -5376,12 +5562,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="87" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K87" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="L87" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="M87" t="s">
         <v>233</v>
@@ -5402,12 +5588,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="88" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K88" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="L88" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="M88" t="s">
         <v>233</v>
@@ -5428,12 +5614,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="89" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K89" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="L89" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="M89" t="s">
         <v>233</v>
@@ -5454,12 +5640,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="90" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K90" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="L90" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="M90" t="s">
         <v>233</v>
@@ -5480,12 +5666,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="91" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K91" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="L91" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="M91" t="s">
         <v>233</v>
@@ -5506,12 +5692,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="92" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K92" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="L92" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="M92" t="s">
         <v>233</v>
@@ -5532,12 +5718,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="93" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K93" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="L93" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="M93" t="s">
         <v>233</v>
@@ -5558,232 +5744,160 @@
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>31</v>
-      </c>
-      <c r="H94" t="s">
-        <v>31</v>
-      </c>
+    <row r="94" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K94" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="L94" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="M94" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="N94" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="O94" t="s">
         <v>36</v>
       </c>
       <c r="P94" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="Q94" t="s">
-        <v>294</v>
+        <v>236</v>
       </c>
       <c r="S94" t="s">
         <v>39</v>
       </c>
-      <c r="U94">
-        <v>-1</v>
-      </c>
-      <c r="V94" t="s">
-        <v>193</v>
-      </c>
-      <c r="W94" t="s">
-        <v>295</v>
-      </c>
-      <c r="X94" t="s">
-        <v>296</v>
-      </c>
-      <c r="Z94" t="s">
-        <v>297</v>
-      </c>
-      <c r="AA94" t="s">
-        <v>297</v>
-      </c>
-      <c r="AB94" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K95" t="s">
+        <v>279</v>
+      </c>
+      <c r="L95" t="s">
+        <v>280</v>
+      </c>
       <c r="M95" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="N95" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="O95" t="s">
         <v>36</v>
       </c>
       <c r="P95" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="Q95" t="s">
-        <v>294</v>
+        <v>236</v>
       </c>
       <c r="S95" t="s">
-        <v>88</v>
-      </c>
-      <c r="X95" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>31</v>
-      </c>
-      <c r="H96" t="s">
-        <v>31</v>
-      </c>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="11:19" x14ac:dyDescent="0.25">
       <c r="K96" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="L96" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="M96" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="N96" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="O96" t="s">
         <v>36</v>
       </c>
       <c r="P96" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="Q96" t="s">
-        <v>294</v>
+        <v>236</v>
       </c>
       <c r="S96" t="s">
         <v>39</v>
       </c>
-      <c r="U96">
-        <v>-1</v>
-      </c>
-      <c r="V96" t="s">
-        <v>193</v>
-      </c>
-      <c r="W96" t="s">
-        <v>295</v>
-      </c>
-      <c r="X96" t="s">
-        <v>296</v>
-      </c>
-      <c r="Z96" t="s">
-        <v>301</v>
-      </c>
-      <c r="AA96" t="s">
-        <v>301</v>
-      </c>
-      <c r="AB96" t="s">
-        <v>298</v>
-      </c>
     </row>
     <row r="97" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K97" t="s">
+        <v>283</v>
+      </c>
+      <c r="L97" t="s">
+        <v>284</v>
+      </c>
       <c r="M97" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="N97" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="O97" t="s">
         <v>36</v>
       </c>
       <c r="P97" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="Q97" t="s">
-        <v>294</v>
+        <v>236</v>
       </c>
       <c r="S97" t="s">
-        <v>88</v>
-      </c>
-      <c r="X97" t="s">
-        <v>296</v>
+        <v>39</v>
       </c>
     </row>
     <row r="98" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>31</v>
-      </c>
-      <c r="H98" t="s">
-        <v>31</v>
-      </c>
       <c r="K98" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="L98" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="M98" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="N98" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="O98" t="s">
         <v>36</v>
       </c>
       <c r="P98" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="Q98" t="s">
-        <v>294</v>
+        <v>236</v>
       </c>
       <c r="S98" t="s">
         <v>39</v>
       </c>
-      <c r="U98">
-        <v>-1</v>
-      </c>
-      <c r="V98" t="s">
-        <v>193</v>
-      </c>
-      <c r="W98" t="s">
-        <v>295</v>
-      </c>
-      <c r="X98" t="s">
-        <v>296</v>
-      </c>
-      <c r="Z98" t="s">
-        <v>304</v>
-      </c>
-      <c r="AA98" t="s">
-        <v>304</v>
-      </c>
-      <c r="AB98" t="s">
-        <v>298</v>
-      </c>
     </row>
     <row r="99" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K99" t="s">
+        <v>287</v>
+      </c>
+      <c r="L99" t="s">
+        <v>288</v>
+      </c>
       <c r="M99" t="s">
-        <v>291</v>
+        <v>233</v>
       </c>
       <c r="N99" t="s">
-        <v>292</v>
+        <v>234</v>
       </c>
       <c r="O99" t="s">
         <v>36</v>
       </c>
       <c r="P99" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="Q99" t="s">
-        <v>294</v>
+        <v>236</v>
       </c>
       <c r="S99" t="s">
-        <v>88</v>
-      </c>
-      <c r="X99" t="s">
-        <v>296</v>
+        <v>39</v>
       </c>
     </row>
     <row r="100" spans="1:32" x14ac:dyDescent="0.25">
@@ -5794,10 +5908,10 @@
         <v>31</v>
       </c>
       <c r="K100" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="L100" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="M100" t="s">
         <v>291</v>
@@ -5830,10 +5944,10 @@
         <v>296</v>
       </c>
       <c r="Z100" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="AA100" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="AB100" t="s">
         <v>298</v>
@@ -5870,10 +5984,10 @@
         <v>31</v>
       </c>
       <c r="K102" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="L102" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="M102" t="s">
         <v>291</v>
@@ -5891,46 +6005,31 @@
         <v>294</v>
       </c>
       <c r="S102" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="U102">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V102" t="s">
         <v>193</v>
       </c>
       <c r="W102" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="X102" t="s">
         <v>296</v>
       </c>
       <c r="Z102" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="AA102" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="AB102" t="s">
         <v>298</v>
       </c>
-      <c r="AF102" t="s">
-        <v>312</v>
-      </c>
     </row>
     <row r="103" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>31</v>
-      </c>
-      <c r="H103" t="s">
-        <v>31</v>
-      </c>
-      <c r="K103" t="s">
-        <v>313</v>
-      </c>
-      <c r="L103" t="s">
-        <v>314</v>
-      </c>
       <c r="M103" t="s">
         <v>291</v>
       </c>
@@ -5949,37 +6048,22 @@
       <c r="S103" t="s">
         <v>88</v>
       </c>
-      <c r="U103">
-        <v>1</v>
-      </c>
-      <c r="V103" t="s">
-        <v>193</v>
-      </c>
-      <c r="W103" t="s">
-        <v>310</v>
-      </c>
       <c r="X103" t="s">
         <v>296</v>
       </c>
-      <c r="Z103" t="s">
-        <v>315</v>
-      </c>
-      <c r="AA103" t="s">
-        <v>315</v>
-      </c>
-      <c r="AB103" t="s">
-        <v>298</v>
-      </c>
-      <c r="AF103" t="s">
-        <v>312</v>
-      </c>
     </row>
     <row r="104" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>31</v>
+      </c>
+      <c r="H104" t="s">
+        <v>31</v>
+      </c>
       <c r="K104" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="L104" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="M104" t="s">
         <v>291</v>
@@ -5999,17 +6083,29 @@
       <c r="S104" t="s">
         <v>39</v>
       </c>
+      <c r="U104">
+        <v>-1</v>
+      </c>
+      <c r="V104" t="s">
+        <v>193</v>
+      </c>
+      <c r="W104" t="s">
+        <v>295</v>
+      </c>
       <c r="X104" t="s">
         <v>296</v>
       </c>
+      <c r="Z104" t="s">
+        <v>304</v>
+      </c>
+      <c r="AA104" t="s">
+        <v>304</v>
+      </c>
+      <c r="AB104" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="105" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K105" t="s">
-        <v>318</v>
-      </c>
-      <c r="L105" t="s">
-        <v>319</v>
-      </c>
       <c r="M105" t="s">
         <v>291</v>
       </c>
@@ -6026,1054 +6122,1129 @@
         <v>294</v>
       </c>
       <c r="S105" t="s">
-        <v>320</v>
+        <v>88</v>
       </c>
       <c r="X105" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="106" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>31</v>
+      </c>
+      <c r="H106" t="s">
+        <v>31</v>
+      </c>
       <c r="K106" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="L106" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="M106" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="N106" t="s">
-        <v>324</v>
+        <v>292</v>
       </c>
       <c r="O106" t="s">
         <v>36</v>
       </c>
       <c r="P106" t="s">
-        <v>325</v>
+        <v>293</v>
       </c>
       <c r="Q106" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="S106" t="s">
         <v>39</v>
       </c>
+      <c r="U106">
+        <v>-1</v>
+      </c>
+      <c r="V106" t="s">
+        <v>193</v>
+      </c>
+      <c r="W106" t="s">
+        <v>295</v>
+      </c>
+      <c r="X106" t="s">
+        <v>296</v>
+      </c>
+      <c r="Z106" t="s">
+        <v>307</v>
+      </c>
+      <c r="AA106" t="s">
+        <v>307</v>
+      </c>
+      <c r="AB106" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="107" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="K107" t="s">
-        <v>327</v>
-      </c>
-      <c r="L107" t="s">
-        <v>328</v>
-      </c>
       <c r="M107" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="N107" t="s">
-        <v>324</v>
+        <v>292</v>
       </c>
       <c r="O107" t="s">
         <v>36</v>
       </c>
       <c r="P107" t="s">
-        <v>325</v>
+        <v>293</v>
       </c>
       <c r="Q107" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="S107" t="s">
-        <v>39</v>
+        <v>88</v>
+      </c>
+      <c r="X107" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="108" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B108" t="s">
+      <c r="A108" t="s">
+        <v>31</v>
+      </c>
+      <c r="H108" t="s">
         <v>31</v>
       </c>
       <c r="K108" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="L108" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
       <c r="M108" t="s">
-        <v>331</v>
+        <v>291</v>
       </c>
       <c r="N108" t="s">
-        <v>332</v>
+        <v>292</v>
       </c>
       <c r="O108" t="s">
         <v>36</v>
       </c>
       <c r="P108" t="s">
-        <v>333</v>
+        <v>293</v>
       </c>
       <c r="Q108" t="s">
-        <v>334</v>
+        <v>294</v>
       </c>
       <c r="S108" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="U108">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="V108" t="s">
-        <v>40</v>
+        <v>193</v>
       </c>
       <c r="W108" t="s">
-        <v>335</v>
+        <v>310</v>
       </c>
       <c r="X108" t="s">
-        <v>336</v>
+        <v>296</v>
+      </c>
+      <c r="Z108" t="s">
+        <v>311</v>
+      </c>
+      <c r="AA108" t="s">
+        <v>311</v>
       </c>
       <c r="AB108" t="s">
-        <v>337</v>
-      </c>
-      <c r="AE108">
-        <v>2</v>
+        <v>298</v>
       </c>
       <c r="AF108" t="s">
-        <v>338</v>
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>31</v>
       </c>
+      <c r="H109" t="s">
+        <v>31</v>
+      </c>
       <c r="K109" t="s">
-        <v>339</v>
+        <v>313</v>
       </c>
       <c r="L109" t="s">
-        <v>340</v>
+        <v>314</v>
       </c>
       <c r="M109" t="s">
-        <v>331</v>
+        <v>291</v>
       </c>
       <c r="N109" t="s">
-        <v>341</v>
+        <v>292</v>
       </c>
       <c r="O109" t="s">
         <v>36</v>
       </c>
       <c r="P109" t="s">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="Q109" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
       <c r="S109" t="s">
-        <v>39</v>
+        <v>88</v>
+      </c>
+      <c r="U109">
+        <v>1</v>
+      </c>
+      <c r="V109" t="s">
+        <v>193</v>
+      </c>
+      <c r="W109" t="s">
+        <v>310</v>
       </c>
       <c r="X109" t="s">
-        <v>344</v>
+        <v>296</v>
+      </c>
+      <c r="Z109" t="s">
+        <v>315</v>
+      </c>
+      <c r="AA109" t="s">
+        <v>315</v>
       </c>
       <c r="AB109" t="s">
-        <v>345</v>
+        <v>298</v>
+      </c>
+      <c r="AF109" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="110" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>31</v>
-      </c>
-      <c r="J110" t="s">
-        <v>31</v>
-      </c>
       <c r="K110" t="s">
-        <v>339</v>
+        <v>316</v>
       </c>
       <c r="L110" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="M110" t="s">
-        <v>331</v>
+        <v>291</v>
       </c>
       <c r="N110" t="s">
-        <v>341</v>
+        <v>292</v>
       </c>
       <c r="O110" t="s">
         <v>36</v>
       </c>
-      <c r="P110">
-        <v>2012</v>
+      <c r="P110" t="s">
+        <v>293</v>
       </c>
       <c r="Q110" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
       <c r="S110" t="s">
         <v>39</v>
       </c>
       <c r="X110" t="s">
-        <v>346</v>
-      </c>
-      <c r="AB110" t="s">
-        <v>347</v>
+        <v>296</v>
       </c>
     </row>
     <row r="111" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>31</v>
-      </c>
-      <c r="E111" t="s">
-        <v>31</v>
-      </c>
       <c r="K111" t="s">
-        <v>348</v>
+        <v>318</v>
       </c>
       <c r="L111" t="s">
-        <v>349</v>
+        <v>319</v>
       </c>
       <c r="M111" t="s">
-        <v>331</v>
+        <v>291</v>
       </c>
       <c r="N111" t="s">
-        <v>341</v>
+        <v>292</v>
       </c>
       <c r="O111" t="s">
         <v>36</v>
       </c>
-      <c r="P111">
-        <v>2012</v>
+      <c r="P111" t="s">
+        <v>293</v>
       </c>
       <c r="Q111" t="s">
-        <v>343</v>
+        <v>294</v>
       </c>
       <c r="S111" t="s">
-        <v>39</v>
+        <v>320</v>
       </c>
       <c r="X111" t="s">
-        <v>346</v>
-      </c>
-      <c r="AB111" t="s">
-        <v>350</v>
+        <v>296</v>
       </c>
     </row>
     <row r="112" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K112" t="s">
-        <v>351</v>
+        <v>321</v>
       </c>
       <c r="L112" t="s">
-        <v>352</v>
+        <v>322</v>
       </c>
       <c r="M112" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="N112" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="O112" t="s">
         <v>36</v>
       </c>
-      <c r="P112">
-        <v>2011</v>
+      <c r="P112" t="s">
+        <v>325</v>
       </c>
       <c r="Q112" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="S112" t="s">
-        <v>88</v>
-      </c>
-      <c r="X112" t="s">
-        <v>344</v>
-      </c>
-      <c r="AB112" t="s">
-        <v>345</v>
+        <v>39</v>
       </c>
     </row>
     <row r="113" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K113" t="s">
-        <v>353</v>
+        <v>327</v>
       </c>
       <c r="L113" t="s">
-        <v>354</v>
+        <v>328</v>
       </c>
       <c r="M113" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="N113" t="s">
-        <v>355</v>
+        <v>324</v>
       </c>
       <c r="O113" t="s">
         <v>36</v>
       </c>
       <c r="P113" t="s">
-        <v>356</v>
+        <v>325</v>
       </c>
       <c r="Q113" t="s">
-        <v>357</v>
+        <v>326</v>
       </c>
       <c r="S113" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>31</v>
+      </c>
       <c r="K114" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
       <c r="L114" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="M114" t="s">
         <v>331</v>
       </c>
       <c r="N114" t="s">
-        <v>360</v>
+        <v>332</v>
       </c>
       <c r="O114" t="s">
         <v>36</v>
       </c>
       <c r="P114" t="s">
-        <v>356</v>
+        <v>333</v>
       </c>
       <c r="Q114" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="S114" t="s">
         <v>39</v>
       </c>
+      <c r="U114">
+        <v>-1</v>
+      </c>
+      <c r="V114" t="s">
+        <v>40</v>
+      </c>
+      <c r="W114" t="s">
+        <v>335</v>
+      </c>
+      <c r="X114" t="s">
+        <v>336</v>
+      </c>
+      <c r="AB114" t="s">
+        <v>337</v>
+      </c>
+      <c r="AE114">
+        <v>2</v>
+      </c>
+      <c r="AF114" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="115" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>31</v>
+      </c>
       <c r="K115" t="s">
-        <v>362</v>
+        <v>339</v>
       </c>
       <c r="L115" t="s">
-        <v>363</v>
+        <v>340</v>
       </c>
       <c r="M115" t="s">
         <v>331</v>
       </c>
       <c r="N115" t="s">
-        <v>364</v>
+        <v>341</v>
       </c>
       <c r="O115" t="s">
         <v>36</v>
       </c>
       <c r="P115" t="s">
-        <v>356</v>
+        <v>342</v>
       </c>
       <c r="Q115" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="S115" t="s">
         <v>39</v>
       </c>
+      <c r="X115" t="s">
+        <v>344</v>
+      </c>
+      <c r="AB115" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="116" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>31</v>
+      </c>
+      <c r="J116" t="s">
+        <v>31</v>
+      </c>
       <c r="K116" t="s">
-        <v>366</v>
+        <v>339</v>
       </c>
       <c r="L116" t="s">
-        <v>367</v>
+        <v>340</v>
       </c>
       <c r="M116" t="s">
         <v>331</v>
       </c>
       <c r="N116" t="s">
-        <v>368</v>
+        <v>341</v>
       </c>
       <c r="O116" t="s">
         <v>36</v>
       </c>
-      <c r="P116" t="s">
-        <v>356</v>
+      <c r="P116">
+        <v>2012</v>
       </c>
       <c r="Q116" t="s">
-        <v>369</v>
+        <v>343</v>
       </c>
       <c r="S116" t="s">
         <v>39</v>
+      </c>
+      <c r="X116" t="s">
+        <v>346</v>
+      </c>
+      <c r="AB116" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>31</v>
       </c>
-      <c r="B117" t="s">
-        <v>31</v>
-      </c>
       <c r="E117" t="s">
         <v>31</v>
       </c>
       <c r="K117" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="L117" t="s">
-        <v>371</v>
+        <v>349</v>
       </c>
       <c r="M117" t="s">
         <v>331</v>
       </c>
       <c r="N117" t="s">
-        <v>372</v>
+        <v>341</v>
       </c>
       <c r="O117" t="s">
         <v>36</v>
       </c>
-      <c r="P117" t="s">
-        <v>97</v>
+      <c r="P117">
+        <v>2012</v>
       </c>
       <c r="Q117" t="s">
-        <v>373</v>
+        <v>343</v>
       </c>
       <c r="S117" t="s">
         <v>39</v>
       </c>
-      <c r="U117">
-        <v>1</v>
-      </c>
-      <c r="V117" t="s">
-        <v>40</v>
-      </c>
-      <c r="W117" t="s">
-        <v>335</v>
-      </c>
       <c r="X117" t="s">
-        <v>374</v>
+        <v>346</v>
       </c>
       <c r="AB117" t="s">
-        <v>375</v>
-      </c>
-      <c r="AD117" t="s">
-        <v>57</v>
+        <v>350</v>
       </c>
     </row>
     <row r="118" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>31</v>
-      </c>
-      <c r="B118" t="s">
-        <v>31</v>
-      </c>
       <c r="K118" t="s">
-        <v>376</v>
+        <v>351</v>
       </c>
       <c r="L118" t="s">
-        <v>377</v>
+        <v>352</v>
       </c>
       <c r="M118" t="s">
         <v>331</v>
       </c>
       <c r="N118" t="s">
-        <v>378</v>
+        <v>341</v>
       </c>
       <c r="O118" t="s">
         <v>36</v>
       </c>
-      <c r="P118" t="s">
-        <v>379</v>
+      <c r="P118">
+        <v>2011</v>
       </c>
       <c r="Q118" t="s">
-        <v>380</v>
+        <v>343</v>
       </c>
       <c r="S118" t="s">
-        <v>39</v>
-      </c>
-      <c r="U118">
-        <v>1</v>
-      </c>
-      <c r="V118" t="s">
-        <v>40</v>
-      </c>
-      <c r="W118" t="s">
-        <v>335</v>
+        <v>88</v>
       </c>
       <c r="X118" t="s">
-        <v>381</v>
-      </c>
-      <c r="Y118" t="s">
-        <v>382</v>
-      </c>
-      <c r="Z118" t="s">
-        <v>383</v>
+        <v>344</v>
       </c>
       <c r="AB118" t="s">
-        <v>384</v>
-      </c>
-      <c r="AD118" t="s">
-        <v>57</v>
+        <v>345</v>
       </c>
     </row>
     <row r="119" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>31</v>
-      </c>
-      <c r="B119" t="s">
-        <v>31</v>
-      </c>
       <c r="K119" t="s">
-        <v>385</v>
+        <v>353</v>
       </c>
       <c r="L119" t="s">
-        <v>386</v>
+        <v>354</v>
       </c>
       <c r="M119" t="s">
         <v>331</v>
       </c>
       <c r="N119" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
       <c r="O119" t="s">
         <v>36</v>
       </c>
       <c r="P119" t="s">
-        <v>379</v>
+        <v>356</v>
       </c>
       <c r="Q119" t="s">
-        <v>380</v>
+        <v>357</v>
       </c>
       <c r="S119" t="s">
         <v>39</v>
-      </c>
-      <c r="U119">
-        <v>1</v>
-      </c>
-      <c r="V119" t="s">
-        <v>40</v>
-      </c>
-      <c r="W119" t="s">
-        <v>335</v>
-      </c>
-      <c r="X119" t="s">
-        <v>381</v>
-      </c>
-      <c r="Y119" t="s">
-        <v>382</v>
-      </c>
-      <c r="Z119" t="s">
-        <v>387</v>
-      </c>
-      <c r="AB119" t="s">
-        <v>384</v>
-      </c>
-      <c r="AD119" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="120" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K120" t="s">
-        <v>388</v>
+        <v>358</v>
       </c>
       <c r="L120" t="s">
-        <v>389</v>
+        <v>359</v>
       </c>
       <c r="M120" t="s">
-        <v>390</v>
+        <v>331</v>
       </c>
       <c r="N120" t="s">
-        <v>391</v>
+        <v>360</v>
       </c>
       <c r="O120" t="s">
         <v>36</v>
       </c>
       <c r="P120" t="s">
-        <v>36</v>
+        <v>356</v>
       </c>
       <c r="Q120" t="s">
-        <v>392</v>
+        <v>361</v>
       </c>
       <c r="S120" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF120" t="s">
-        <v>393</v>
+        <v>39</v>
       </c>
     </row>
     <row r="121" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K121" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
       <c r="L121" t="s">
-        <v>394</v>
+        <v>363</v>
       </c>
       <c r="M121" t="s">
-        <v>390</v>
+        <v>331</v>
       </c>
       <c r="N121" t="s">
-        <v>391</v>
+        <v>364</v>
       </c>
       <c r="O121" t="s">
         <v>36</v>
       </c>
       <c r="P121" t="s">
-        <v>36</v>
+        <v>356</v>
       </c>
       <c r="Q121" t="s">
-        <v>392</v>
+        <v>365</v>
       </c>
       <c r="S121" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
     <row r="122" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K122" t="s">
-        <v>388</v>
+        <v>366</v>
       </c>
       <c r="L122" t="s">
-        <v>395</v>
+        <v>367</v>
       </c>
       <c r="M122" t="s">
-        <v>390</v>
+        <v>331</v>
       </c>
       <c r="N122" t="s">
-        <v>391</v>
+        <v>368</v>
       </c>
       <c r="O122" t="s">
         <v>36</v>
       </c>
       <c r="P122" t="s">
-        <v>36</v>
+        <v>356</v>
       </c>
       <c r="Q122" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
       <c r="S122" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
     <row r="123" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>31</v>
+      </c>
+      <c r="B123" t="s">
+        <v>31</v>
+      </c>
+      <c r="E123" t="s">
+        <v>31</v>
+      </c>
       <c r="K123" t="s">
-        <v>388</v>
+        <v>370</v>
       </c>
       <c r="L123" t="s">
-        <v>396</v>
+        <v>371</v>
       </c>
       <c r="M123" t="s">
-        <v>390</v>
+        <v>331</v>
       </c>
       <c r="N123" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="O123" t="s">
         <v>36</v>
       </c>
       <c r="P123" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="Q123" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
       <c r="S123" t="s">
-        <v>88</v>
+        <v>39</v>
+      </c>
+      <c r="U123">
+        <v>1</v>
+      </c>
+      <c r="V123" t="s">
+        <v>40</v>
+      </c>
+      <c r="W123" t="s">
+        <v>335</v>
+      </c>
+      <c r="X123" t="s">
+        <v>374</v>
+      </c>
+      <c r="AB123" t="s">
+        <v>375</v>
+      </c>
+      <c r="AD123" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="124" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>31</v>
       </c>
-      <c r="E124" t="s">
+      <c r="B124" t="s">
         <v>31</v>
       </c>
       <c r="K124" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
       <c r="L124" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="M124" t="s">
-        <v>399</v>
+        <v>331</v>
       </c>
       <c r="N124" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="O124" t="s">
         <v>36</v>
       </c>
       <c r="P124" t="s">
-        <v>401</v>
+        <v>379</v>
       </c>
       <c r="Q124" t="s">
-        <v>402</v>
-      </c>
-      <c r="R124" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="S124" t="s">
         <v>39</v>
       </c>
-      <c r="T124" t="s">
-        <v>404</v>
+      <c r="U124">
+        <v>1</v>
+      </c>
+      <c r="V124" t="s">
+        <v>40</v>
+      </c>
+      <c r="W124" t="s">
+        <v>335</v>
       </c>
       <c r="X124" t="s">
-        <v>405</v>
+        <v>381</v>
+      </c>
+      <c r="Y124" t="s">
+        <v>382</v>
+      </c>
+      <c r="Z124" t="s">
+        <v>383</v>
       </c>
       <c r="AB124" t="s">
-        <v>406</v>
-      </c>
-      <c r="AC124" t="s">
-        <v>129</v>
+        <v>384</v>
+      </c>
+      <c r="AD124" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>31</v>
       </c>
-      <c r="E125" t="s">
-        <v>31</v>
-      </c>
-      <c r="J125" t="s">
+      <c r="B125" t="s">
         <v>31</v>
       </c>
       <c r="K125" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="L125" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="M125" t="s">
-        <v>399</v>
+        <v>331</v>
       </c>
       <c r="N125" t="s">
-        <v>400</v>
+        <v>378</v>
       </c>
       <c r="O125" t="s">
         <v>36</v>
       </c>
       <c r="P125" t="s">
-        <v>70</v>
+        <v>379</v>
       </c>
       <c r="Q125" t="s">
-        <v>402</v>
-      </c>
-      <c r="R125" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
       <c r="S125" t="s">
         <v>39</v>
       </c>
-      <c r="T125" t="s">
-        <v>404</v>
+      <c r="U125">
+        <v>1</v>
+      </c>
+      <c r="V125" t="s">
+        <v>40</v>
+      </c>
+      <c r="W125" t="s">
+        <v>335</v>
       </c>
       <c r="X125" t="s">
-        <v>407</v>
+        <v>381</v>
+      </c>
+      <c r="Y125" t="s">
+        <v>382</v>
+      </c>
+      <c r="Z125" t="s">
+        <v>387</v>
       </c>
       <c r="AB125" t="s">
-        <v>406</v>
-      </c>
-      <c r="AC125" t="s">
-        <v>129</v>
+        <v>384</v>
+      </c>
+      <c r="AD125" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>31</v>
-      </c>
-      <c r="E126" t="s">
-        <v>31</v>
-      </c>
       <c r="K126" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="L126" t="s">
-        <v>409</v>
+        <v>389</v>
       </c>
       <c r="M126" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="N126" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="O126" t="s">
         <v>36</v>
       </c>
       <c r="P126" t="s">
-        <v>411</v>
+        <v>36</v>
       </c>
       <c r="Q126" t="s">
-        <v>402</v>
-      </c>
-      <c r="R126" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="S126" t="s">
-        <v>39</v>
-      </c>
-      <c r="T126" t="s">
-        <v>404</v>
-      </c>
-      <c r="X126" t="s">
-        <v>412</v>
-      </c>
-      <c r="AB126" t="s">
-        <v>406</v>
+        <v>88</v>
+      </c>
+      <c r="AF126" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>31</v>
-      </c>
-      <c r="E127" t="s">
-        <v>31</v>
-      </c>
-      <c r="J127" t="s">
-        <v>31</v>
-      </c>
       <c r="K127" t="s">
-        <v>408</v>
+        <v>388</v>
       </c>
       <c r="L127" t="s">
-        <v>409</v>
+        <v>394</v>
       </c>
       <c r="M127" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="N127" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
       <c r="O127" t="s">
         <v>36</v>
       </c>
-      <c r="P127">
-        <v>2012</v>
+      <c r="P127" t="s">
+        <v>36</v>
       </c>
       <c r="Q127" t="s">
-        <v>402</v>
-      </c>
-      <c r="R127" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="S127" t="s">
-        <v>39</v>
-      </c>
-      <c r="T127" t="s">
-        <v>404</v>
-      </c>
-      <c r="X127" t="s">
-        <v>413</v>
-      </c>
-      <c r="AB127" t="s">
-        <v>406</v>
+        <v>88</v>
       </c>
     </row>
     <row r="128" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K128" t="s">
-        <v>370</v>
+        <v>388</v>
       </c>
       <c r="L128" t="s">
-        <v>371</v>
+        <v>395</v>
       </c>
       <c r="M128" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="N128" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
       <c r="O128" t="s">
         <v>36</v>
       </c>
       <c r="P128" t="s">
-        <v>415</v>
+        <v>36</v>
       </c>
       <c r="Q128" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="S128" t="s">
-        <v>39</v>
-      </c>
-      <c r="T128" t="s">
-        <v>404</v>
-      </c>
-      <c r="U128">
-        <v>1</v>
-      </c>
-      <c r="V128" t="s">
-        <v>40</v>
-      </c>
-      <c r="W128" t="s">
-        <v>335</v>
-      </c>
-      <c r="X128" t="s">
-        <v>416</v>
-      </c>
-      <c r="AB128" t="s">
-        <v>406</v>
-      </c>
-      <c r="AD128" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF128" t="s">
-        <v>417</v>
+        <v>88</v>
       </c>
     </row>
     <row r="129" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K129" t="s">
-        <v>418</v>
+        <v>388</v>
       </c>
       <c r="L129" t="s">
-        <v>419</v>
+        <v>396</v>
       </c>
       <c r="M129" t="s">
-        <v>420</v>
+        <v>390</v>
       </c>
       <c r="N129" t="s">
-        <v>421</v>
+        <v>391</v>
       </c>
       <c r="O129" t="s">
         <v>36</v>
       </c>
       <c r="P129" t="s">
-        <v>422</v>
+        <v>36</v>
       </c>
       <c r="Q129" t="s">
-        <v>423</v>
-      </c>
-      <c r="R129" t="s">
-        <v>424</v>
+        <v>392</v>
       </c>
       <c r="S129" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
     </row>
     <row r="130" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>31</v>
+      </c>
+      <c r="E130" t="s">
+        <v>31</v>
+      </c>
       <c r="K130" t="s">
-        <v>425</v>
+        <v>397</v>
       </c>
       <c r="L130" t="s">
-        <v>426</v>
+        <v>398</v>
       </c>
       <c r="M130" t="s">
-        <v>420</v>
+        <v>399</v>
+      </c>
+      <c r="N130" t="s">
+        <v>400</v>
       </c>
       <c r="O130" t="s">
         <v>36</v>
       </c>
       <c r="P130" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="Q130" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="R130" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="S130" t="s">
         <v>39</v>
       </c>
+      <c r="T130" t="s">
+        <v>404</v>
+      </c>
+      <c r="X130" t="s">
+        <v>405</v>
+      </c>
+      <c r="AB130" t="s">
+        <v>406</v>
+      </c>
+      <c r="AC130" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="131" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>31</v>
+      </c>
+      <c r="E131" t="s">
+        <v>31</v>
+      </c>
+      <c r="J131" t="s">
+        <v>31</v>
+      </c>
       <c r="K131" t="s">
-        <v>427</v>
+        <v>397</v>
       </c>
       <c r="L131" t="s">
-        <v>428</v>
+        <v>398</v>
       </c>
       <c r="M131" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="N131" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="O131" t="s">
         <v>36</v>
       </c>
       <c r="P131" t="s">
-        <v>422</v>
+        <v>70</v>
       </c>
       <c r="Q131" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="R131" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="S131" t="s">
         <v>39</v>
       </c>
+      <c r="T131" t="s">
+        <v>404</v>
+      </c>
+      <c r="X131" t="s">
+        <v>407</v>
+      </c>
+      <c r="AB131" t="s">
+        <v>406</v>
+      </c>
+      <c r="AC131" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="132" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>31</v>
+      </c>
+      <c r="E132" t="s">
+        <v>31</v>
+      </c>
       <c r="K132" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
       <c r="L132" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
       <c r="M132" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="N132" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
       <c r="O132" t="s">
         <v>36</v>
       </c>
       <c r="P132" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="Q132" t="s">
-        <v>432</v>
+        <v>402</v>
       </c>
       <c r="R132" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="S132" t="s">
         <v>39</v>
       </c>
+      <c r="T132" t="s">
+        <v>404</v>
+      </c>
+      <c r="X132" t="s">
+        <v>412</v>
+      </c>
+      <c r="AB132" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="133" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>31</v>
+      </c>
+      <c r="E133" t="s">
+        <v>31</v>
+      </c>
+      <c r="J133" t="s">
+        <v>31</v>
+      </c>
       <c r="K133" t="s">
-        <v>433</v>
+        <v>408</v>
       </c>
       <c r="L133" t="s">
-        <v>434</v>
+        <v>409</v>
       </c>
       <c r="M133" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="N133" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
       <c r="O133" t="s">
         <v>36</v>
       </c>
-      <c r="P133" t="s">
-        <v>422</v>
+      <c r="P133">
+        <v>2012</v>
       </c>
       <c r="Q133" t="s">
-        <v>432</v>
+        <v>402</v>
       </c>
       <c r="R133" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="S133" t="s">
         <v>39</v>
+      </c>
+      <c r="T133" t="s">
+        <v>404</v>
+      </c>
+      <c r="X133" t="s">
+        <v>413</v>
+      </c>
+      <c r="AB133" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="134" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K134" t="s">
-        <v>435</v>
+        <v>370</v>
       </c>
       <c r="L134" t="s">
-        <v>436</v>
+        <v>371</v>
       </c>
       <c r="M134" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="N134" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="O134" t="s">
         <v>36</v>
       </c>
       <c r="P134" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="Q134" t="s">
-        <v>432</v>
-      </c>
-      <c r="R134" t="s">
-        <v>424</v>
+        <v>402</v>
       </c>
       <c r="S134" t="s">
         <v>39</v>
+      </c>
+      <c r="T134" t="s">
+        <v>404</v>
+      </c>
+      <c r="U134">
+        <v>1</v>
+      </c>
+      <c r="V134" t="s">
+        <v>40</v>
+      </c>
+      <c r="W134" t="s">
+        <v>335</v>
+      </c>
+      <c r="X134" t="s">
+        <v>416</v>
+      </c>
+      <c r="AB134" t="s">
+        <v>406</v>
+      </c>
+      <c r="AD134" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF134" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="135" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K135" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="L135" t="s">
-        <v>437</v>
+        <v>419</v>
       </c>
       <c r="M135" t="s">
         <v>420</v>
       </c>
       <c r="N135" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="O135" t="s">
         <v>36</v>
@@ -7082,7 +7253,7 @@
         <v>422</v>
       </c>
       <c r="Q135" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="R135" t="s">
         <v>424</v>
@@ -7093,17 +7264,14 @@
     </row>
     <row r="136" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K136" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="L136" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="M136" t="s">
         <v>420</v>
       </c>
-      <c r="N136" t="s">
-        <v>431</v>
-      </c>
       <c r="O136" t="s">
         <v>36</v>
       </c>
@@ -7111,7 +7279,7 @@
         <v>422</v>
       </c>
       <c r="Q136" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="R136" t="s">
         <v>424</v>
@@ -7122,16 +7290,16 @@
     </row>
     <row r="137" spans="1:32" x14ac:dyDescent="0.25">
       <c r="K137" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="L137" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="M137" t="s">
         <v>420</v>
       </c>
       <c r="N137" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="O137" t="s">
         <v>36</v>
@@ -7140,7 +7308,7 @@
         <v>422</v>
       </c>
       <c r="Q137" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="R137" t="s">
         <v>424</v>
@@ -7150,96 +7318,84 @@
       </c>
     </row>
     <row r="138" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>31</v>
-      </c>
-      <c r="F138" t="s">
-        <v>31</v>
-      </c>
       <c r="K138" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="L138" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="M138" t="s">
-        <v>442</v>
+        <v>420</v>
       </c>
       <c r="N138" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="O138" t="s">
         <v>36</v>
       </c>
       <c r="P138" t="s">
-        <v>445</v>
+        <v>422</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>432</v>
       </c>
       <c r="R138" t="s">
-        <v>446</v>
+        <v>424</v>
       </c>
       <c r="S138" t="s">
-        <v>447</v>
-      </c>
-      <c r="V138" t="s">
-        <v>448</v>
-      </c>
-      <c r="AB138" t="s">
-        <v>449</v>
+        <v>39</v>
       </c>
     </row>
     <row r="139" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>31</v>
-      </c>
       <c r="K139" t="s">
-        <v>68</v>
+        <v>433</v>
       </c>
       <c r="L139" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
       <c r="M139" t="s">
-        <v>451</v>
+        <v>420</v>
       </c>
       <c r="N139" t="s">
-        <v>69</v>
-      </c>
-      <c r="P139">
-        <v>2013</v>
+        <v>431</v>
+      </c>
+      <c r="O139" t="s">
+        <v>36</v>
+      </c>
+      <c r="P139" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>432</v>
+      </c>
+      <c r="R139" t="s">
+        <v>424</v>
       </c>
       <c r="S139" t="s">
-        <v>452</v>
-      </c>
-      <c r="V139" t="s">
-        <v>193</v>
-      </c>
-      <c r="AB139" t="s">
-        <v>453</v>
+        <v>39</v>
       </c>
     </row>
     <row r="140" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>31</v>
-      </c>
-      <c r="H140" t="s">
-        <v>31</v>
-      </c>
-      <c r="I140">
-        <v>100</v>
-      </c>
       <c r="K140" t="s">
-        <v>454</v>
+        <v>435</v>
       </c>
       <c r="L140" t="s">
-        <v>455</v>
+        <v>436</v>
       </c>
       <c r="M140" t="s">
-        <v>456</v>
-      </c>
-      <c r="P140">
-        <v>2013</v>
+        <v>420</v>
+      </c>
+      <c r="N140" t="s">
+        <v>431</v>
+      </c>
+      <c r="O140" t="s">
+        <v>36</v>
+      </c>
+      <c r="P140" t="s">
+        <v>422</v>
       </c>
       <c r="Q140" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="R140" t="s">
         <v>424</v>
@@ -7247,58 +7403,28 @@
       <c r="S140" t="s">
         <v>39</v>
       </c>
-      <c r="U140">
-        <v>1</v>
-      </c>
-      <c r="V140" t="s">
-        <v>40</v>
-      </c>
-      <c r="W140" t="s">
-        <v>125</v>
-      </c>
-      <c r="X140" t="s">
-        <v>458</v>
-      </c>
-      <c r="Z140" t="s">
-        <v>459</v>
-      </c>
-      <c r="AA140" t="s">
-        <v>460</v>
-      </c>
-      <c r="AB140" t="s">
-        <v>461</v>
-      </c>
-      <c r="AD140" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF140" t="s">
-        <v>462</v>
-      </c>
     </row>
     <row r="141" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>31</v>
-      </c>
-      <c r="H141" t="s">
-        <v>31</v>
-      </c>
-      <c r="I141">
-        <v>100</v>
-      </c>
       <c r="K141" t="s">
-        <v>463</v>
+        <v>427</v>
       </c>
       <c r="L141" t="s">
-        <v>464</v>
+        <v>437</v>
       </c>
       <c r="M141" t="s">
-        <v>456</v>
-      </c>
-      <c r="P141">
-        <v>2013</v>
+        <v>420</v>
+      </c>
+      <c r="N141" t="s">
+        <v>431</v>
+      </c>
+      <c r="O141" t="s">
+        <v>36</v>
+      </c>
+      <c r="P141" t="s">
+        <v>422</v>
       </c>
       <c r="Q141" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="R141" t="s">
         <v>424</v>
@@ -7306,58 +7432,28 @@
       <c r="S141" t="s">
         <v>39</v>
       </c>
-      <c r="U141">
-        <v>1</v>
-      </c>
-      <c r="V141" t="s">
-        <v>40</v>
-      </c>
-      <c r="W141" t="s">
-        <v>125</v>
-      </c>
-      <c r="X141" t="s">
-        <v>458</v>
-      </c>
-      <c r="Z141" t="s">
-        <v>465</v>
-      </c>
-      <c r="AA141" t="s">
-        <v>466</v>
-      </c>
-      <c r="AB141" t="s">
-        <v>461</v>
-      </c>
-      <c r="AD141" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF141" t="s">
-        <v>462</v>
-      </c>
     </row>
     <row r="142" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>31</v>
-      </c>
-      <c r="H142" t="s">
-        <v>31</v>
-      </c>
-      <c r="I142">
-        <v>100</v>
-      </c>
       <c r="K142" t="s">
-        <v>467</v>
+        <v>438</v>
       </c>
       <c r="L142" t="s">
-        <v>468</v>
+        <v>439</v>
       </c>
       <c r="M142" t="s">
-        <v>456</v>
-      </c>
-      <c r="P142">
-        <v>2013</v>
+        <v>420</v>
+      </c>
+      <c r="N142" t="s">
+        <v>431</v>
+      </c>
+      <c r="O142" t="s">
+        <v>36</v>
+      </c>
+      <c r="P142" t="s">
+        <v>422</v>
       </c>
       <c r="Q142" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="R142" t="s">
         <v>424</v>
@@ -7365,58 +7461,28 @@
       <c r="S142" t="s">
         <v>39</v>
       </c>
-      <c r="U142">
-        <v>1</v>
-      </c>
-      <c r="V142" t="s">
-        <v>40</v>
-      </c>
-      <c r="W142" t="s">
-        <v>125</v>
-      </c>
-      <c r="X142" t="s">
-        <v>458</v>
-      </c>
-      <c r="Z142" t="s">
-        <v>469</v>
-      </c>
-      <c r="AA142" t="s">
-        <v>470</v>
-      </c>
-      <c r="AB142" t="s">
-        <v>461</v>
-      </c>
-      <c r="AD142" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF142" t="s">
-        <v>462</v>
-      </c>
     </row>
     <row r="143" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>31</v>
-      </c>
-      <c r="H143" t="s">
-        <v>31</v>
-      </c>
-      <c r="I143">
-        <v>100</v>
-      </c>
       <c r="K143" t="s">
-        <v>471</v>
+        <v>440</v>
       </c>
       <c r="L143" t="s">
-        <v>472</v>
+        <v>441</v>
       </c>
       <c r="M143" t="s">
-        <v>456</v>
-      </c>
-      <c r="P143">
-        <v>2013</v>
+        <v>420</v>
+      </c>
+      <c r="N143" t="s">
+        <v>431</v>
+      </c>
+      <c r="O143" t="s">
+        <v>36</v>
+      </c>
+      <c r="P143" t="s">
+        <v>422</v>
       </c>
       <c r="Q143" t="s">
-        <v>457</v>
+        <v>432</v>
       </c>
       <c r="R143" t="s">
         <v>424</v>
@@ -7424,154 +7490,77 @@
       <c r="S143" t="s">
         <v>39</v>
       </c>
-      <c r="U143">
-        <v>1</v>
-      </c>
-      <c r="V143" t="s">
-        <v>40</v>
-      </c>
-      <c r="W143" t="s">
-        <v>125</v>
-      </c>
-      <c r="X143" t="s">
-        <v>458</v>
-      </c>
-      <c r="Z143" t="s">
-        <v>473</v>
-      </c>
-      <c r="AA143" t="s">
-        <v>474</v>
-      </c>
-      <c r="AB143" t="s">
-        <v>461</v>
-      </c>
-      <c r="AD143" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF143" t="s">
-        <v>462</v>
-      </c>
     </row>
     <row r="144" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>31</v>
       </c>
-      <c r="H144" t="s">
-        <v>31</v>
-      </c>
-      <c r="I144">
-        <v>100</v>
+      <c r="F144" t="s">
+        <v>31</v>
       </c>
       <c r="K144" t="s">
-        <v>475</v>
+        <v>442</v>
       </c>
       <c r="L144" t="s">
-        <v>476</v>
+        <v>443</v>
       </c>
       <c r="M144" t="s">
-        <v>456</v>
-      </c>
-      <c r="P144">
-        <v>2013</v>
-      </c>
-      <c r="Q144" t="s">
-        <v>457</v>
+        <v>442</v>
+      </c>
+      <c r="N144" t="s">
+        <v>444</v>
+      </c>
+      <c r="O144" t="s">
+        <v>36</v>
+      </c>
+      <c r="P144" t="s">
+        <v>445</v>
       </c>
       <c r="R144" t="s">
-        <v>424</v>
+        <v>446</v>
       </c>
       <c r="S144" t="s">
-        <v>39</v>
-      </c>
-      <c r="U144">
-        <v>1</v>
+        <v>447</v>
       </c>
       <c r="V144" t="s">
-        <v>40</v>
-      </c>
-      <c r="W144" t="s">
-        <v>125</v>
-      </c>
-      <c r="X144" t="s">
-        <v>458</v>
-      </c>
-      <c r="Z144" t="s">
-        <v>477</v>
-      </c>
-      <c r="AA144" t="s">
-        <v>478</v>
+        <v>448</v>
       </c>
       <c r="AB144" t="s">
-        <v>461</v>
-      </c>
-      <c r="AD144" t="s">
-        <v>57</v>
-      </c>
-      <c r="AF144" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>31</v>
       </c>
-      <c r="B145" t="s">
-        <v>31</v>
-      </c>
-      <c r="D145" t="s">
-        <v>121</v>
-      </c>
-      <c r="H145" t="s">
-        <v>31</v>
-      </c>
       <c r="K145" t="s">
-        <v>479</v>
+        <v>68</v>
       </c>
       <c r="L145" t="s">
-        <v>480</v>
+        <v>450</v>
       </c>
       <c r="M145" t="s">
-        <v>456</v>
+        <v>451</v>
+      </c>
+      <c r="N145" t="s">
+        <v>69</v>
       </c>
       <c r="P145">
         <v>2013</v>
       </c>
-      <c r="Q145" t="s">
-        <v>457</v>
-      </c>
-      <c r="R145" t="s">
-        <v>424</v>
-      </c>
       <c r="S145" t="s">
-        <v>39</v>
-      </c>
-      <c r="U145">
-        <v>1</v>
+        <v>452</v>
       </c>
       <c r="V145" t="s">
-        <v>40</v>
-      </c>
-      <c r="W145" t="s">
-        <v>125</v>
-      </c>
-      <c r="X145" t="s">
-        <v>458</v>
-      </c>
-      <c r="Z145" t="s">
-        <v>481</v>
-      </c>
-      <c r="AA145" t="s">
-        <v>481</v>
+        <v>193</v>
       </c>
       <c r="AB145" t="s">
-        <v>461</v>
-      </c>
-      <c r="AF145" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix akamai 2013 percentage import
</commit_message>
<xml_diff>
--- a/db/sources.xlsx
+++ b/db/sources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="0" windowWidth="27540" windowHeight="14310"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="27540" windowHeight="14310"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -2327,8 +2327,8 @@
   <dimension ref="A1:AF145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,6 +2754,9 @@
       <c r="B7" t="s">
         <v>31</v>
       </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
       <c r="J7" t="s">
         <v>31</v>
       </c>
@@ -2868,6 +2871,9 @@
       </c>
       <c r="B9" t="s">
         <v>31</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
       </c>
       <c r="J9" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
#8219 - update bb pricing data to include Iran; #8502 - flip google default weight
</commit_message>
<xml_diff>
--- a/db/sources.xlsx
+++ b/db/sources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="0" windowWidth="27540" windowHeight="14310"/>
+    <workbookView xWindow="5040" yWindow="0" windowWidth="27540" windowHeight="14310"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -2326,9 +2326,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U55" sqref="U55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4318,7 +4318,7 @@
         <v>39</v>
       </c>
       <c r="U49">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V49" t="s">
         <v>40</v>
@@ -4377,7 +4377,7 @@
         <v>39</v>
       </c>
       <c r="U50">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V50" t="s">
         <v>40</v>
@@ -4436,7 +4436,7 @@
         <v>39</v>
       </c>
       <c r="U51">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V51" t="s">
         <v>40</v>
@@ -4495,7 +4495,7 @@
         <v>39</v>
       </c>
       <c r="U52">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V52" t="s">
         <v>40</v>
@@ -4554,7 +4554,7 @@
         <v>39</v>
       </c>
       <c r="U53">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V53" t="s">
         <v>40</v>
@@ -4616,7 +4616,7 @@
         <v>39</v>
       </c>
       <c r="U54">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V54" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
#9693 - begin API indicators
</commit_message>
<xml_diff>
--- a/db/sources.xlsx
+++ b/db/sources.xlsx
@@ -2376,14 +2376,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>

</xml_diff>

<commit_message>
#9693 - indicator for external data
</commit_message>
<xml_diff>
--- a/db/sources.xlsx
+++ b/db/sources.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="0" windowWidth="17490" windowHeight="9345"/>
+    <workbookView xWindow="3780" yWindow="0" windowWidth="17490" windowHeight="9345"/>
   </bookViews>
   <sheets>
     <sheet name="sources" sheetId="1" r:id="rId1"/>
@@ -2068,9 +2068,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AF145" totalsRowShown="0">
   <autoFilter ref="A1:AF145">
     <filterColumn colId="0">
-      <filters>
-        <filter val="y"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="32">
@@ -2377,8 +2377,8 @@
   <dimension ref="A1:AF145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A133" sqref="A133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7536,7 +7536,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="144" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>100</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="145" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>100</v>
       </c>

</xml_diff>